<commit_message>
add bug reports document
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC02_Register/TC02_Register_TestCase.xlsx
+++ b/Documents/1_TestCases/TC02_Register/TC02_Register_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC02_Register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C57586E-2EC3-497D-B274-0B6102321E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB880BB-8EE3-4CBB-9843-FD5D8CB6384D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add register test case, add employeeListPage object, update docs
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC02_Register/TC02_Register_TestCase.xlsx
+++ b/Documents/1_TestCases/TC02_Register/TC02_Register_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC02_Register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB880BB-8EE3-4CBB-9843-FD5D8CB6384D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA289B0-D3D2-4072-B9CF-510013A778EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Test ID</t>
   </si>
@@ -183,9 +183,6 @@
 3.Validation error should arise about max character length.</t>
   </si>
   <si>
-    <t>Manual or Automated</t>
-  </si>
-  <si>
     <t>Verify that the newly added employee appears in the employee list/table after submission.</t>
   </si>
   <si>
@@ -199,6 +196,27 @@
   </si>
   <si>
     <t>Field should have visible placeholders.</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Automated
+Bug: Register_B01</t>
+  </si>
+  <si>
+    <t>Automated
+Bug: Register_B03</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Manual
+Bug: Register_B02</t>
   </si>
 </sst>
 </file>
@@ -631,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +709,12 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -708,6 +732,12 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -725,6 +755,12 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -742,6 +778,12 @@
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -759,6 +801,12 @@
       <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -776,6 +824,12 @@
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -791,10 +845,13 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="90" x14ac:dyDescent="0.25">
@@ -802,16 +859,19 @@
         <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>43</v>
+      <c r="I10" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="60" x14ac:dyDescent="0.25">

</xml_diff>